<commit_message>
Novo Up arquivo editado
</commit_message>
<xml_diff>
--- a/Documentos/Mapeamento - Geral - ODBC.xlsx
+++ b/Documentos/Mapeamento - Geral - ODBC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\int.matheus\Desktop\DW\Data-Warehouse\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7457D1A3-AD53-403E-87C0-2E1E285B5CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11ABC24-E2AE-4917-A7A0-15A79F9DF3FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0D9869C1-0C4A-4AC6-8A9B-8CE4CB7120E4}"/>
   </bookViews>
@@ -1428,9 +1428,6 @@
     <t>52.179.19.141</t>
   </si>
   <si>
-    <t>Actyon- New</t>
-  </si>
-  <si>
     <t>45.77.94.104</t>
   </si>
   <si>
@@ -1546,6 +1543,9 @@
   </si>
   <si>
     <t>MySQL ODBC 8.4 ANSI Driver</t>
+  </si>
+  <si>
+    <t>Actyon-New</t>
   </si>
 </sst>
 </file>
@@ -1675,7 +1675,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1832,7 +1832,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1914,6 +1914,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1932,16 +1944,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2265,7 +2268,7 @@
   <dimension ref="B1:X58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="P13" sqref="P12:P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2276,7 +2279,7 @@
     <col min="4" max="4" width="18.44140625" style="1" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" style="1" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="18.88671875" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5546875" style="1" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
@@ -2337,11 +2340,11 @@
       <c r="L3" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="M3" s="39" t="s">
+      <c r="M3" s="33" t="s">
         <v>443</v>
       </c>
-      <c r="N3" s="39" t="s">
-        <v>496</v>
+      <c r="N3" s="33" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="4" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
@@ -2357,13 +2360,13 @@
       <c r="E4" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="F4" s="42" t="s">
+      <c r="F4" s="36" t="s">
         <v>445</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H4" s="41">
+      <c r="H4" s="35">
         <v>1433</v>
       </c>
       <c r="I4" s="6" t="s">
@@ -2382,7 +2385,7 @@
         <v>442</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="5" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
@@ -2396,15 +2399,15 @@
         <v>451</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>463</v>
-      </c>
-      <c r="F5" s="42" t="s">
+        <v>462</v>
+      </c>
+      <c r="F5" s="36" t="s">
         <v>225</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="H5" s="41">
+      <c r="H5" s="35">
         <v>3306</v>
       </c>
       <c r="I5" s="6" t="s">
@@ -2418,10 +2421,10 @@
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="6" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="6" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
@@ -2435,15 +2438,15 @@
         <v>451</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>463</v>
-      </c>
-      <c r="F6" s="42" t="s">
+        <v>462</v>
+      </c>
+      <c r="F6" s="36" t="s">
         <v>225</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="H6" s="41">
+      <c r="H6" s="35">
         <v>3306</v>
       </c>
       <c r="I6" s="6" t="s">
@@ -2457,14 +2460,14 @@
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="6" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="7" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="43" t="s">
         <v>78</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -2476,20 +2479,20 @@
       <c r="E7" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="F7" s="42" t="s">
+      <c r="F7" s="36" t="s">
         <v>225</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H7" s="41">
+      <c r="H7" s="35">
         <v>1433</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>80</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="K7" s="26" t="s">
         <v>218</v>
@@ -2498,14 +2501,14 @@
         <v>114</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="8" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="43" t="s">
         <v>82</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -2517,20 +2520,20 @@
       <c r="E8" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="F8" s="42" t="s">
+      <c r="F8" s="36" t="s">
         <v>225</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H8" s="41">
+      <c r="H8" s="35">
         <v>1433</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>457</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="K8" s="26" t="s">
         <v>218</v>
@@ -2539,14 +2542,14 @@
         <v>116</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="9" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="34" t="s">
         <v>72</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -2558,91 +2561,91 @@
       <c r="E9" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="36" t="s">
         <v>225</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H9" s="41">
+      <c r="H9" s="35">
         <v>1433</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>75</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="K9" s="26" t="s">
         <v>219</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="10" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="34" t="s">
+        <v>499</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>460</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>461</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F10" s="42" t="s">
+      <c r="F10" s="36" t="s">
         <v>225</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H10" s="41">
+      <c r="H10" s="35">
         <v>1433</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>355</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="K10" s="26" t="s">
         <v>440</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="6" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="11" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="34" t="s">
         <v>354</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>441</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="42" t="s">
+      <c r="F11" s="36" t="s">
         <v>300</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H11" s="41">
+      <c r="H11" s="35">
         <v>1433</v>
       </c>
       <c r="I11" s="6" t="s">
@@ -2656,32 +2659,32 @@
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="6" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="12" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="40" t="s">
-        <v>472</v>
+      <c r="B12" s="34" t="s">
+        <v>471</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="42" t="s">
+      <c r="F12" s="36" t="s">
         <v>66</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H12" s="41">
+      <c r="H12" s="35">
         <v>1433</v>
       </c>
       <c r="I12" s="6" t="s">
@@ -2697,32 +2700,32 @@
         <v>150</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="13" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="40" t="s">
-        <v>473</v>
+      <c r="B13" s="44" t="s">
+        <v>472</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="42" t="s">
+      <c r="F13" s="36" t="s">
         <v>67</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H13" s="41">
+      <c r="H13" s="35">
         <v>1433</v>
       </c>
       <c r="I13" s="6" t="s">
@@ -2738,32 +2741,32 @@
         <v>152</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="14" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="40" t="s">
-        <v>473</v>
+      <c r="B14" s="44" t="s">
+        <v>472</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="42" t="s">
+      <c r="F14" s="36" t="s">
         <v>67</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H14" s="41">
+      <c r="H14" s="35">
         <v>1433</v>
       </c>
       <c r="I14" s="6" t="s">
@@ -2779,32 +2782,32 @@
         <v>153</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="15" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="40" t="s">
-        <v>473</v>
+      <c r="B15" s="44" t="s">
+        <v>472</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="36" t="s">
         <v>67</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H15" s="41">
+      <c r="H15" s="35">
         <v>1433</v>
       </c>
       <c r="I15" s="6" t="s">
@@ -2820,32 +2823,32 @@
         <v>155</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="16" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="40" t="s">
-        <v>473</v>
+      <c r="B16" s="44" t="s">
+        <v>472</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F16" s="42" t="s">
+      <c r="F16" s="36" t="s">
         <v>67</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H16" s="41">
+      <c r="H16" s="35">
         <v>1433</v>
       </c>
       <c r="I16" s="6" t="s">
@@ -2861,32 +2864,32 @@
         <v>157</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="N16" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="17" spans="2:24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="34" t="s">
+        <v>473</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>474</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>471</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>475</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="42" t="s">
+      <c r="F17" s="36" t="s">
         <v>67</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H17" s="41">
+      <c r="H17" s="35">
         <v>1433</v>
       </c>
       <c r="I17" s="6" t="s">
@@ -2902,32 +2905,32 @@
         <v>206</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="18" spans="2:24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="34" t="s">
+        <v>473</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>474</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>471</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>475</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F18" s="42" t="s">
+      <c r="F18" s="36" t="s">
         <v>67</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H18" s="41">
+      <c r="H18" s="35">
         <v>1433</v>
       </c>
       <c r="I18" s="6" t="s">
@@ -2943,32 +2946,32 @@
         <v>207</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="N18" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="19" spans="2:24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="34" t="s">
+        <v>473</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>474</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>471</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>475</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F19" s="42" t="s">
+      <c r="F19" s="36" t="s">
         <v>67</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H19" s="41">
+      <c r="H19" s="35">
         <v>1433</v>
       </c>
       <c r="I19" s="6" t="s">
@@ -2984,32 +2987,32 @@
         <v>208</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N19" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="20" spans="2:24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="34" t="s">
+        <v>473</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>474</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>471</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>475</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F20" s="42" t="s">
+      <c r="F20" s="36" t="s">
         <v>67</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H20" s="41">
+      <c r="H20" s="35">
         <v>1433</v>
       </c>
       <c r="I20" s="6" t="s">
@@ -3025,15 +3028,15 @@
         <v>209</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="N20" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="21" spans="2:24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="40" t="s">
-        <v>466</v>
+      <c r="B21" s="34" t="s">
+        <v>465</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>22</v>
@@ -3042,22 +3045,22 @@
         <v>112</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>463</v>
-      </c>
-      <c r="F21" s="42" t="s">
-        <v>470</v>
+        <v>462</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>469</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H21" s="41">
+      <c r="H21" s="35">
         <v>1433</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="K21" s="26" t="s">
         <v>24</v>
@@ -3066,15 +3069,15 @@
         <v>214</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="N21" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="22" spans="2:24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="40" t="s">
-        <v>468</v>
+      <c r="B22" s="34" t="s">
+        <v>467</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>211</v>
@@ -3083,22 +3086,22 @@
         <v>112</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>463</v>
-      </c>
-      <c r="F22" s="42" t="s">
-        <v>470</v>
+        <v>462</v>
+      </c>
+      <c r="F22" s="36" t="s">
+        <v>469</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H22" s="41">
+      <c r="H22" s="35">
         <v>1433</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="K22" s="26" t="s">
         <v>24</v>
@@ -3107,15 +3110,15 @@
         <v>215</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="23" spans="2:24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="40" t="s">
-        <v>466</v>
+      <c r="B23" s="34" t="s">
+        <v>465</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>212</v>
@@ -3124,22 +3127,22 @@
         <v>112</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>463</v>
-      </c>
-      <c r="F23" s="42" t="s">
-        <v>470</v>
+        <v>462</v>
+      </c>
+      <c r="F23" s="36" t="s">
+        <v>469</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H23" s="41">
+      <c r="H23" s="35">
         <v>1433</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="K23" s="26" t="s">
         <v>24</v>
@@ -3148,15 +3151,15 @@
         <v>216</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="N23" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="24" spans="2:24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="40" t="s">
-        <v>467</v>
+      <c r="B24" s="34" t="s">
+        <v>466</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>211</v>
@@ -3165,22 +3168,22 @@
         <v>112</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>463</v>
-      </c>
-      <c r="F24" s="42" t="s">
+        <v>462</v>
+      </c>
+      <c r="F24" s="36" t="s">
         <v>300</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H24" s="41">
+      <c r="H24" s="35">
         <v>1433</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>358</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="K24" s="26" t="s">
         <v>357</v>
@@ -3189,10 +3192,10 @@
         <v>217</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="N24" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="25" spans="2:24" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3335,9 +3338,11 @@
     <hyperlink ref="C19" r:id="rId10" tooltip="https://10.10.220.101/" display="https://10.10.220.101/" xr:uid="{439A4C9C-8289-4EF2-A99F-EFA5E470C4CB}"/>
     <hyperlink ref="C18" r:id="rId11" tooltip="https://10.10.220.101/" display="https://10.10.220.101/" xr:uid="{E4F6DE81-164F-44C0-9878-944B61CB5B91}"/>
     <hyperlink ref="C17" r:id="rId12" tooltip="https://10.10.220.101/" display="https://10.10.220.101/" xr:uid="{4892D943-755A-40B9-AD66-EDC6C0E4B9E8}"/>
+    <hyperlink ref="K12" r:id="rId13" xr:uid="{8FCB2007-1587-450A-AE38-062DE161BD57}"/>
+    <hyperlink ref="K13" r:id="rId14" xr:uid="{EFD06393-F3D2-452C-879B-68D9A79958B3}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 
@@ -3418,7 +3423,7 @@
       <c r="M3" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="N3" s="39" t="s">
+      <c r="N3" s="33" t="s">
         <v>443</v>
       </c>
     </row>
@@ -4832,51 +4837,51 @@
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10"/>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="40" t="s">
         <v>177</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="37" t="s">
+      <c r="I3" s="41" t="s">
         <v>268</v>
       </c>
-      <c r="J3" s="38"/>
-      <c r="K3" s="37" t="s">
+      <c r="J3" s="42"/>
+      <c r="K3" s="41" t="s">
         <v>271</v>
       </c>
-      <c r="L3" s="38"/>
+      <c r="L3" s="42"/>
       <c r="M3"/>
-      <c r="N3" s="33" t="s">
+      <c r="N3" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="O3" s="34"/>
-      <c r="P3" s="35" t="s">
+      <c r="O3" s="38"/>
+      <c r="P3" s="39" t="s">
         <v>204</v>
       </c>
-      <c r="Q3" s="35"/>
+      <c r="Q3" s="39"/>
       <c r="R3" s="11"/>
     </row>
     <row r="4" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
       <c r="I4" s="15" t="s">
         <v>269</v>
       </c>
@@ -5584,29 +5589,29 @@
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="10"/>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="40" t="s">
         <v>320</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="40" t="s">
         <v>315</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="40" t="s">
         <v>321</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="40" t="s">
         <v>308</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
       <c r="J3" s="23"/>
-      <c r="K3" s="36" t="s">
+      <c r="K3" s="40" t="s">
         <v>309</v>
       </c>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
       <c r="P3" s="11"/>
       <c r="Q3" s="1"/>
       <c r="S3" s="2" t="s">
@@ -5619,9 +5624,9 @@
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="10"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
       <c r="F4" s="15" t="s">
         <v>239</v>
       </c>
@@ -7754,7 +7759,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8116,38 +8121,38 @@
     </row>
     <row r="3" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10"/>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="40" t="s">
         <v>400</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="40" t="s">
         <v>177</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="40" t="s">
         <v>409</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="40" t="s">
         <v>93</v>
       </c>
       <c r="J3" s="10"/>
     </row>
     <row r="4" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
       <c r="J4" s="10"/>
     </row>
     <row r="5" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Novo Up Todos os env's configurados
</commit_message>
<xml_diff>
--- a/Documentos/Mapeamento - Geral - ODBC.xlsx
+++ b/Documentos/Mapeamento - Geral - ODBC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\int.matheus\Desktop\DW\Data-Warehouse\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11ABC24-E2AE-4917-A7A0-15A79F9DF3FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDC82E9-4B4E-462A-A660-FFCC4761F78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0D9869C1-0C4A-4AC6-8A9B-8CE4CB7120E4}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="501">
   <si>
     <t>IP</t>
   </si>
@@ -1546,6 +1546,9 @@
   </si>
   <si>
     <t>Actyon-New</t>
+  </si>
+  <si>
+    <t>45.77.164.133</t>
   </si>
 </sst>
 </file>
@@ -1926,6 +1929,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1944,10 +1950,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2268,7 +2271,7 @@
   <dimension ref="B1:X58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P13" sqref="P12:P13"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2348,10 +2351,10 @@
       </c>
     </row>
     <row r="4" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="44" t="s">
         <v>458</v>
       </c>
       <c r="D4" s="6" t="s">
@@ -2389,10 +2392,10 @@
       </c>
     </row>
     <row r="5" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="34" t="s">
         <v>448</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="44" t="s">
         <v>228</v>
       </c>
       <c r="D5" s="6" t="s">
@@ -2428,10 +2431,10 @@
       </c>
     </row>
     <row r="6" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="34" t="s">
         <v>449</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="44" t="s">
         <v>228</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -2467,10 +2470,10 @@
       </c>
     </row>
     <row r="7" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="44" t="s">
         <v>79</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -2508,10 +2511,10 @@
       </c>
     </row>
     <row r="8" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="44" t="s">
         <v>456</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -2552,7 +2555,7 @@
       <c r="B9" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="44" t="s">
         <v>459</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -2591,7 +2594,7 @@
       <c r="B10" s="34" t="s">
         <v>499</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="44" t="s">
         <v>460</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -2630,8 +2633,8 @@
       <c r="B11" s="34" t="s">
         <v>354</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>441</v>
+      <c r="C11" s="44" t="s">
+        <v>500</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>474</v>
@@ -2669,7 +2672,7 @@
       <c r="B12" s="34" t="s">
         <v>471</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="44" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="6" t="s">
@@ -2707,10 +2710,10 @@
       </c>
     </row>
     <row r="13" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="37" t="s">
         <v>472</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="44" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -2748,10 +2751,10 @@
       </c>
     </row>
     <row r="14" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="37" t="s">
         <v>472</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="44" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="6" t="s">
@@ -2789,10 +2792,10 @@
       </c>
     </row>
     <row r="15" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="37" t="s">
         <v>472</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="44" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="6" t="s">
@@ -2830,10 +2833,10 @@
       </c>
     </row>
     <row r="16" spans="2:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="37" t="s">
         <v>472</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="44" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="6" t="s">
@@ -2874,7 +2877,7 @@
       <c r="B17" s="34" t="s">
         <v>473</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="44" t="s">
         <v>470</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -2915,7 +2918,7 @@
       <c r="B18" s="34" t="s">
         <v>473</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="44" t="s">
         <v>470</v>
       </c>
       <c r="D18" s="6" t="s">
@@ -2956,7 +2959,7 @@
       <c r="B19" s="34" t="s">
         <v>473</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="44" t="s">
         <v>470</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -2997,7 +3000,7 @@
       <c r="B20" s="34" t="s">
         <v>473</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="44" t="s">
         <v>470</v>
       </c>
       <c r="D20" s="6" t="s">
@@ -3038,7 +3041,7 @@
       <c r="B21" s="34" t="s">
         <v>465</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="44" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="6" t="s">
@@ -3079,7 +3082,7 @@
       <c r="B22" s="34" t="s">
         <v>467</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="44" t="s">
         <v>211</v>
       </c>
       <c r="D22" s="6" t="s">
@@ -3120,7 +3123,7 @@
       <c r="B23" s="34" t="s">
         <v>465</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="44" t="s">
         <v>212</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -3161,7 +3164,7 @@
       <c r="B24" s="34" t="s">
         <v>466</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="44" t="s">
         <v>211</v>
       </c>
       <c r="D24" s="6" t="s">
@@ -3340,9 +3343,10 @@
     <hyperlink ref="C17" r:id="rId12" tooltip="https://10.10.220.101/" display="https://10.10.220.101/" xr:uid="{4892D943-755A-40B9-AD66-EDC6C0E4B9E8}"/>
     <hyperlink ref="K12" r:id="rId13" xr:uid="{8FCB2007-1587-450A-AE38-062DE161BD57}"/>
     <hyperlink ref="K13" r:id="rId14" xr:uid="{EFD06393-F3D2-452C-879B-68D9A79958B3}"/>
+    <hyperlink ref="K10" r:id="rId15" xr:uid="{6A9E3A8F-6C09-45ED-B0B7-E63DE6389CB8}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 
@@ -4837,51 +4841,51 @@
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10"/>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="40" t="s">
+      <c r="H3" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="42" t="s">
         <v>268</v>
       </c>
-      <c r="J3" s="42"/>
-      <c r="K3" s="41" t="s">
+      <c r="J3" s="43"/>
+      <c r="K3" s="42" t="s">
         <v>271</v>
       </c>
-      <c r="L3" s="42"/>
+      <c r="L3" s="43"/>
       <c r="M3"/>
-      <c r="N3" s="37" t="s">
+      <c r="N3" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="O3" s="38"/>
-      <c r="P3" s="39" t="s">
+      <c r="O3" s="39"/>
+      <c r="P3" s="40" t="s">
         <v>204</v>
       </c>
-      <c r="Q3" s="39"/>
+      <c r="Q3" s="40"/>
       <c r="R3" s="11"/>
     </row>
     <row r="4" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
       <c r="I4" s="15" t="s">
         <v>269</v>
       </c>
@@ -5589,29 +5593,29 @@
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="10"/>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="41" t="s">
         <v>320</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="41" t="s">
         <v>315</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="41" t="s">
         <v>321</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="41" t="s">
         <v>308</v>
       </c>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
       <c r="J3" s="23"/>
-      <c r="K3" s="40" t="s">
+      <c r="K3" s="41" t="s">
         <v>309</v>
       </c>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
       <c r="P3" s="11"/>
       <c r="Q3" s="1"/>
       <c r="S3" s="2" t="s">
@@ -5624,9 +5628,9 @@
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="10"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
       <c r="F4" s="15" t="s">
         <v>239</v>
       </c>
@@ -8121,38 +8125,38 @@
     </row>
     <row r="3" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10"/>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="41" t="s">
         <v>400</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="40" t="s">
+      <c r="H3" s="41" t="s">
         <v>409</v>
       </c>
-      <c r="I3" s="40" t="s">
+      <c r="I3" s="41" t="s">
         <v>93</v>
       </c>
       <c r="J3" s="10"/>
     </row>
     <row r="4" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
       <c r="J4" s="10"/>
     </row>
     <row r="5" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Novo Up Módulos criados
</commit_message>
<xml_diff>
--- a/Documentos/Mapeamento - Geral - ODBC.xlsx
+++ b/Documentos/Mapeamento - Geral - ODBC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\int.matheus\Desktop\DW\Data-Warehouse\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDC82E9-4B4E-462A-A660-FFCC4761F78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21E6C2D-F136-43F4-B5DA-34CA18C9A7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0D9869C1-0C4A-4AC6-8A9B-8CE4CB7120E4}"/>
   </bookViews>
@@ -1932,6 +1932,9 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1948,9 +1951,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2271,22 +2271,22 @@
   <dimension ref="B1:X58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="0.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" style="1" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="18.44140625" style="1" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" style="1" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="18.88671875" style="1" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="7.5546875" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.77734375" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16.77734375" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" style="1" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="21.6640625" style="1" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="21.6640625" style="1" customWidth="1"/>
     <col min="14" max="14" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
@@ -2354,7 +2354,7 @@
       <c r="B4" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="38" t="s">
         <v>458</v>
       </c>
       <c r="D4" s="6" t="s">
@@ -2395,7 +2395,7 @@
       <c r="B5" s="34" t="s">
         <v>448</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="38" t="s">
         <v>228</v>
       </c>
       <c r="D5" s="6" t="s">
@@ -2434,7 +2434,7 @@
       <c r="B6" s="34" t="s">
         <v>449</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="38" t="s">
         <v>228</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -2473,7 +2473,7 @@
       <c r="B7" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="38" t="s">
         <v>79</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -2514,7 +2514,7 @@
       <c r="B8" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="38" t="s">
         <v>456</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -2555,7 +2555,7 @@
       <c r="B9" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="38" t="s">
         <v>459</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -2594,7 +2594,7 @@
       <c r="B10" s="34" t="s">
         <v>499</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="38" t="s">
         <v>460</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -2633,7 +2633,7 @@
       <c r="B11" s="34" t="s">
         <v>354</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="38" t="s">
         <v>500</v>
       </c>
       <c r="D11" s="6" t="s">
@@ -2672,7 +2672,7 @@
       <c r="B12" s="34" t="s">
         <v>471</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="38" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="6" t="s">
@@ -2713,7 +2713,7 @@
       <c r="B13" s="37" t="s">
         <v>472</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="38" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -2754,7 +2754,7 @@
       <c r="B14" s="37" t="s">
         <v>472</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="38" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="6" t="s">
@@ -2795,7 +2795,7 @@
       <c r="B15" s="37" t="s">
         <v>472</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="38" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="6" t="s">
@@ -2836,7 +2836,7 @@
       <c r="B16" s="37" t="s">
         <v>472</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="38" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="6" t="s">
@@ -2877,7 +2877,7 @@
       <c r="B17" s="34" t="s">
         <v>473</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="38" t="s">
         <v>470</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -2918,7 +2918,7 @@
       <c r="B18" s="34" t="s">
         <v>473</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="38" t="s">
         <v>470</v>
       </c>
       <c r="D18" s="6" t="s">
@@ -2959,7 +2959,7 @@
       <c r="B19" s="34" t="s">
         <v>473</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="38" t="s">
         <v>470</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -3000,7 +3000,7 @@
       <c r="B20" s="34" t="s">
         <v>473</v>
       </c>
-      <c r="C20" s="44" t="s">
+      <c r="C20" s="38" t="s">
         <v>470</v>
       </c>
       <c r="D20" s="6" t="s">
@@ -3041,7 +3041,7 @@
       <c r="B21" s="34" t="s">
         <v>465</v>
       </c>
-      <c r="C21" s="44" t="s">
+      <c r="C21" s="38" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="6" t="s">
@@ -3082,7 +3082,7 @@
       <c r="B22" s="34" t="s">
         <v>467</v>
       </c>
-      <c r="C22" s="44" t="s">
+      <c r="C22" s="38" t="s">
         <v>211</v>
       </c>
       <c r="D22" s="6" t="s">
@@ -3123,7 +3123,7 @@
       <c r="B23" s="34" t="s">
         <v>465</v>
       </c>
-      <c r="C23" s="44" t="s">
+      <c r="C23" s="38" t="s">
         <v>212</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -3164,7 +3164,7 @@
       <c r="B24" s="34" t="s">
         <v>466</v>
       </c>
-      <c r="C24" s="44" t="s">
+      <c r="C24" s="38" t="s">
         <v>211</v>
       </c>
       <c r="D24" s="6" t="s">
@@ -4841,51 +4841,51 @@
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10"/>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="42" t="s">
         <v>177</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="43" t="s">
         <v>268</v>
       </c>
-      <c r="J3" s="43"/>
-      <c r="K3" s="42" t="s">
+      <c r="J3" s="44"/>
+      <c r="K3" s="43" t="s">
         <v>271</v>
       </c>
-      <c r="L3" s="43"/>
+      <c r="L3" s="44"/>
       <c r="M3"/>
-      <c r="N3" s="38" t="s">
+      <c r="N3" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="O3" s="39"/>
-      <c r="P3" s="40" t="s">
+      <c r="O3" s="40"/>
+      <c r="P3" s="41" t="s">
         <v>204</v>
       </c>
-      <c r="Q3" s="40"/>
+      <c r="Q3" s="41"/>
       <c r="R3" s="11"/>
     </row>
     <row r="4" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
       <c r="I4" s="15" t="s">
         <v>269</v>
       </c>
@@ -5593,29 +5593,29 @@
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="10"/>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="42" t="s">
         <v>320</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="42" t="s">
         <v>315</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="42" t="s">
         <v>321</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="42" t="s">
         <v>308</v>
       </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
       <c r="J3" s="23"/>
-      <c r="K3" s="41" t="s">
+      <c r="K3" s="42" t="s">
         <v>309</v>
       </c>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
       <c r="P3" s="11"/>
       <c r="Q3" s="1"/>
       <c r="S3" s="2" t="s">
@@ -5628,9 +5628,9 @@
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="10"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="15" t="s">
         <v>239</v>
       </c>
@@ -8125,38 +8125,38 @@
     </row>
     <row r="3" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10"/>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="42" t="s">
         <v>400</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="42" t="s">
         <v>177</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="42" t="s">
         <v>409</v>
       </c>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="42" t="s">
         <v>93</v>
       </c>
       <c r="J3" s="10"/>
     </row>
     <row r="4" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
       <c r="J4" s="10"/>
     </row>
     <row r="5" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>